<commit_message>
balance de enlance bien hecho
</commit_message>
<xml_diff>
--- a/M7/CODIGOS/resultados_satélites.xlsx
+++ b/M7/CODIGOS/resultados_satélites.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,29 +446,24 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Distancia (km)</t>
+          <t>Distancia Uplink mx (km)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Distancia Downlink mx (km)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Uplink Eb/No (dB)</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Downlink Eb/No (dB)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Uplink EIRP (dBW)</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Downlink EIRP (dBW)</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -478,19 +473,16 @@
         <v>17</v>
       </c>
       <c r="C2" t="n">
-        <v>3398.999852897908</v>
+        <v>7248.583046900511</v>
       </c>
       <c r="D2" t="n">
-        <v>7.256716402375734</v>
+        <v>11233.88175375904</v>
       </c>
       <c r="E2" t="n">
-        <v>14.26906703980765</v>
+        <v>0.6786769385847222</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="G2" t="n">
-        <v>-12</v>
+        <v>3.885492990715338</v>
       </c>
     </row>
     <row r="3">
@@ -501,19 +493,16 @@
         <v>17</v>
       </c>
       <c r="C3" t="n">
-        <v>3398.999852897908</v>
+        <v>7248.583046900511</v>
       </c>
       <c r="D3" t="n">
-        <v>7.256716402375734</v>
+        <v>11233.88175375904</v>
       </c>
       <c r="E3" t="n">
-        <v>14.26906703980765</v>
+        <v>0.6786769385847222</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="G3" t="n">
-        <v>-12</v>
+        <v>3.885492990715338</v>
       </c>
     </row>
     <row r="4">
@@ -524,19 +513,16 @@
         <v>69</v>
       </c>
       <c r="C4" t="n">
-        <v>3398.999852897908</v>
+        <v>7248.583046900511</v>
       </c>
       <c r="D4" t="n">
-        <v>7.256716402375734</v>
+        <v>11233.88175375904</v>
       </c>
       <c r="E4" t="n">
-        <v>14.26906703980765</v>
+        <v>0.6786769385847222</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="G4" t="n">
-        <v>-12</v>
+        <v>3.885492990715338</v>
       </c>
     </row>
     <row r="5">
@@ -547,19 +533,16 @@
         <v>17</v>
       </c>
       <c r="C5" t="n">
-        <v>3398.999852897908</v>
+        <v>7248.583046900511</v>
       </c>
       <c r="D5" t="n">
-        <v>7.256716402375734</v>
+        <v>11233.88175375904</v>
       </c>
       <c r="E5" t="n">
-        <v>14.26906703980765</v>
+        <v>0.6786769385847222</v>
       </c>
       <c r="F5" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="G5" t="n">
-        <v>-12</v>
+        <v>3.885492990715338</v>
       </c>
     </row>
     <row r="6">
@@ -570,19 +553,16 @@
         <v>69</v>
       </c>
       <c r="C6" t="n">
-        <v>3398.999852897908</v>
+        <v>7248.583046900511</v>
       </c>
       <c r="D6" t="n">
-        <v>7.256716402375734</v>
+        <v>11233.88175375904</v>
       </c>
       <c r="E6" t="n">
-        <v>14.26906703980765</v>
+        <v>0.6786769385847222</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="G6" t="n">
-        <v>-12</v>
+        <v>3.885492990715338</v>
       </c>
     </row>
     <row r="7">
@@ -593,19 +573,16 @@
         <v>17</v>
       </c>
       <c r="C7" t="n">
-        <v>3398.999852897908</v>
+        <v>7248.583046900511</v>
       </c>
       <c r="D7" t="n">
-        <v>7.256716402375734</v>
+        <v>11233.88175375904</v>
       </c>
       <c r="E7" t="n">
-        <v>14.26906703980765</v>
+        <v>0.6786769385847222</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="G7" t="n">
-        <v>-12</v>
+        <v>3.885492990715338</v>
       </c>
     </row>
     <row r="8">
@@ -616,19 +593,16 @@
         <v>69</v>
       </c>
       <c r="C8" t="n">
-        <v>3398.999852897908</v>
+        <v>7248.583046900511</v>
       </c>
       <c r="D8" t="n">
-        <v>7.256716402375734</v>
+        <v>11233.88175375904</v>
       </c>
       <c r="E8" t="n">
-        <v>14.26906703980765</v>
+        <v>0.6786769385847222</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="G8" t="n">
-        <v>-12</v>
+        <v>3.885492990715338</v>
       </c>
     </row>
     <row r="9">
@@ -639,19 +613,16 @@
         <v>17</v>
       </c>
       <c r="C9" t="n">
-        <v>3398.999852897908</v>
+        <v>7248.583046900511</v>
       </c>
       <c r="D9" t="n">
-        <v>7.256716402375734</v>
+        <v>11233.88175375904</v>
       </c>
       <c r="E9" t="n">
-        <v>14.26906703980765</v>
+        <v>0.6786769385847222</v>
       </c>
       <c r="F9" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="G9" t="n">
-        <v>-12</v>
+        <v>3.885492990715338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>